<commit_message>
End to end code changes for subjects, semester results, faculty list etc.
</commit_message>
<xml_diff>
--- a/cis-util/data/faculty_details.xlsx
+++ b/cis-util/data/faculty_details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Personal\code\DSCE\CeninfoSys\data\Telecom_Chethan\Telecom_Chethan\Community\Faculty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Personal\code\DSCE\CeninfoSys\trunk\cis-util\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,85 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
-  <si>
-    <t>Dr. A R Aswatha</t>
-  </si>
-  <si>
-    <t>Dr. H C Srinivasaiah</t>
-  </si>
-  <si>
-    <t>Dr. Dr. Devaraju</t>
-  </si>
-  <si>
-    <t>Dr. Ganashree T S</t>
-  </si>
-  <si>
-    <t>Dr. Sayed Abdulhayan</t>
-  </si>
-  <si>
-    <t>Mrs. Manjula Devi T H</t>
-  </si>
-  <si>
-    <t>Mrs. Priti S Pavale</t>
-  </si>
-  <si>
-    <t>Mr. Vinod B Durdi</t>
-  </si>
-  <si>
-    <t>Mrs. Rajeswari P</t>
-  </si>
-  <si>
-    <t>Mrs. Nagarathna</t>
-  </si>
-  <si>
-    <t>Mrs. Sri Vidya B V</t>
-  </si>
-  <si>
-    <t>Mr. Saravana Kumar</t>
-  </si>
-  <si>
-    <t>Mr. Jayanth C</t>
-  </si>
-  <si>
-    <t>Mrs. Anitha Suresh</t>
-  </si>
-  <si>
-    <t>Mr. Santhosh B</t>
-  </si>
-  <si>
-    <t>Ms. Shashikala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs. Smitha Sasi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Kiran Kumar T </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mrs. Pushpa B R </t>
-  </si>
-  <si>
-    <t>Mr. Mahesh Dali</t>
-  </si>
-  <si>
-    <t>Mrs. Deepthi Raj</t>
-  </si>
-  <si>
-    <t>Mr Sandeep K V</t>
-  </si>
-  <si>
-    <t>Mr. Vivek Raj</t>
-  </si>
-  <si>
-    <t>Mr. Chetan Umadi</t>
-  </si>
-  <si>
-    <t>Mr. H Vinod Kumar</t>
-  </si>
-  <si>
-    <t>Mr. M M Hiremath</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
   <si>
     <t>Harsha L</t>
   </si>
@@ -322,6 +244,96 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Dr</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>A R Aswatha</t>
+  </si>
+  <si>
+    <t>H C Srinivasaiah</t>
+  </si>
+  <si>
+    <t>Ganashree T S</t>
+  </si>
+  <si>
+    <t>Sayed Abdulhayan</t>
+  </si>
+  <si>
+    <t>Manjula Devi T H</t>
+  </si>
+  <si>
+    <t>Priti S Pavale</t>
+  </si>
+  <si>
+    <t>Vinod B Durdi</t>
+  </si>
+  <si>
+    <t>Rajeswari P</t>
+  </si>
+  <si>
+    <t>Nagarathna</t>
+  </si>
+  <si>
+    <t>Sri Vidya B V</t>
+  </si>
+  <si>
+    <t>Saravana Kumar</t>
+  </si>
+  <si>
+    <t>Jayanth C</t>
+  </si>
+  <si>
+    <t>Anitha Suresh</t>
+  </si>
+  <si>
+    <t>Shashikala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smitha Sasi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiran Kumar T </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pushpa B R </t>
+  </si>
+  <si>
+    <t>Mahesh Dali</t>
+  </si>
+  <si>
+    <t>Deepthi Raj</t>
+  </si>
+  <si>
+    <t>Sandeep K V</t>
+  </si>
+  <si>
+    <t>Vivek Raj</t>
+  </si>
+  <si>
+    <t>Chetan Umadi</t>
+  </si>
+  <si>
+    <t>H Vinod Kumar</t>
+  </si>
+  <si>
+    <t>M M Hiremath</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Devaraju R</t>
   </si>
 </sst>
 </file>
@@ -760,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -777,786 +789,888 @@
     <col min="7" max="7" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D1" s="3">
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2">
         <v>8277144999</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2">
         <v>9880636776</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2">
         <v>9886675917</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D4" s="2">
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="G4" s="2">
         <v>9945747810</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2">
         <v>9986096513</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3">
         <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2">
         <v>9480591528</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2">
         <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2">
         <v>9845506478</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3">
         <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="G8" s="2">
         <v>9900100605</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2">
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2">
         <v>9986013606</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3">
         <v>14</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2">
         <v>9916990322</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2">
         <v>9741016644</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D12" s="12">
         <v>11</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="G12" s="2">
         <v>9611807758</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2">
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="G13" s="2">
         <v>9886049585</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D14" s="12">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="G14" s="2">
         <v>9845326201</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2">
         <v>9</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="G15" s="2">
         <v>9742084353</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2">
         <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="G16" s="2">
         <v>8884555975</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2">
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="G17" s="2">
         <v>9945800645</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2">
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="G18" s="2">
         <v>9900123562</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2">
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2">
         <v>9731212662</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2">
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="G20" s="2">
         <v>9945707654</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2">
         <v>5</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="G21" s="2">
         <v>9986762618</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
         <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="G22" s="2">
         <v>9945748005</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2">
         <v>2</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="G23" s="2">
         <v>9900451126</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="G24" s="2">
         <v>9620765977</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2">
         <v>2</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="G25" s="2">
         <v>9972243407</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2">
         <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="G26" s="2">
         <v>8095280253</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G28" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D29" s="2">
         <v>0</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G29" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G32" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G33" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>